<commit_message>
Fix Lesson 6 LoLN
</commit_message>
<xml_diff>
--- a/docs/Data/TwinsDiabetes.xlsx
+++ b/docs/Data/TwinsDiabetes.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10323"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ghsaund/Documents/GitHub/BYUI_M221_Book_Sandbox/Data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68D23936-46C9-514E-A6D3-5084227A01CA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="8400" windowHeight="2400"/>
+    <workbookView xWindow="2240" yWindow="7060" windowWidth="17820" windowHeight="15420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,15 +21,90 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
+  <si>
+    <t>Twin</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>NonDiabeticHeight</t>
+  </si>
+  <si>
+    <t>DiabeticHeight</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Researchers measured the heights of</t>
+  </si>
+  <si>
+    <t>young identical twins at the time one</t>
+  </si>
+  <si>
+    <t>(and only one) of the twins was</t>
+  </si>
+  <si>
+    <t>diagnosed with insulin-dependent</t>
+  </si>
+  <si>
+    <t>diabetes. The data represent the</t>
+  </si>
+  <si>
+    <t>heights in cm.</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Hoskins PJ, Leslie RD, Pyke DA.</t>
+  </si>
+  <si>
+    <t>Height at diagnosis of diabetes in children:</t>
+  </si>
+  <si>
+    <t>a study in identical twins.</t>
+  </si>
+  <si>
+    <t>Br Med J (Clin Res Ed).</t>
+  </si>
+  <si>
+    <t>1985 Jan 26;290(6464):278-80.</t>
+  </si>
+  <si>
+    <t>doi: 10.1136/bmj.290.6464.278.</t>
+  </si>
+  <si>
+    <t>PMID: 3917783; PMCID: PMC1417583.</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF201F1E"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -49,19 +130,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="19" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -108,7 +193,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -140,9 +225,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -174,6 +277,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -349,341 +470,346 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" s="0" outlineLevel="0">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Twin</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Age</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Gender</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>NonDiabeticHeight</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>DiabeticHeight</t>
-        </is>
-      </c>
-    </row>
-    <row r="2" spans="1:5" s="0" outlineLevel="0">
-      <c r="A2" t="n">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="n">
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
         <v>14.3</v>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>F</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2">
         <v>157.5</v>
       </c>
-      <c r="E2" t="n">
-        <v>155.0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" s="0" outlineLevel="0">
-      <c r="A3" t="n">
+      <c r="E2">
+        <v>155</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="n">
+      <c r="B3">
         <v>14.1</v>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>F</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>160.0</v>
-      </c>
-      <c r="E3" t="n">
-        <v>158.7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" s="0" outlineLevel="0">
-      <c r="A4" t="n">
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>160</v>
+      </c>
+      <c r="E3">
+        <v>158.69999999999999</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="n">
+      <c r="B4">
         <v>12.6</v>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>F</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
-        <v>153.7</v>
-      </c>
-      <c r="E4" t="n">
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>153.69999999999999</v>
+      </c>
+      <c r="E4">
         <v>149.9</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" s="0" outlineLevel="0">
-      <c r="A5" t="n">
+      <c r="F4" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" t="n">
+      <c r="B5">
         <v>15.1</v>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5">
         <v>172.7</v>
       </c>
-      <c r="E5" t="n">
+      <c r="E5">
         <v>168.9</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" s="0" outlineLevel="0">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="n">
+      <c r="F5" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
         <v>11.1</v>
       </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>137.8</v>
-      </c>
-      <c r="E6" t="n">
-        <v>130.7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" s="0" outlineLevel="0">
-      <c r="A7" t="n">
+      <c r="C6" t="s">
         <v>6</v>
       </c>
-      <c r="B7" t="n">
+      <c r="D6">
+        <v>137.80000000000001</v>
+      </c>
+      <c r="E6">
+        <v>130.69999999999999</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
         <v>18.5</v>
       </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>F</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>162.0</v>
-      </c>
-      <c r="E7" t="n">
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>162</v>
+      </c>
+      <c r="E7">
         <v>159.5</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" s="0" outlineLevel="0">
-      <c r="A8" t="n">
+      <c r="F7" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" t="n">
+      <c r="B8">
         <v>10.9</v>
       </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="D8" t="n">
-        <v>142.2</v>
-      </c>
-      <c r="E8" t="n">
-        <v>139.7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" s="0" outlineLevel="0">
-      <c r="A9" t="n">
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8">
+        <v>142.19999999999999</v>
+      </c>
+      <c r="E8">
+        <v>139.69999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" t="n">
+      <c r="B9">
         <v>8.6</v>
       </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>F</t>
-        </is>
-      </c>
-      <c r="D9" t="n">
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9">
         <v>125.7</v>
       </c>
-      <c r="E9" t="n">
+      <c r="E9">
         <v>121.7</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" s="0" outlineLevel="0">
-      <c r="A10" t="n">
+      <c r="F9" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" t="n">
-        <v>4.1</v>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="D10" t="n">
-        <v>99.0</v>
-      </c>
-      <c r="E10" t="n">
-        <v>99.0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" s="0" outlineLevel="0">
-      <c r="A11" t="n">
+      <c r="B10">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10">
+        <v>99</v>
+      </c>
+      <c r="E10">
+        <v>99</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" t="n">
-        <v>4.6</v>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>F</t>
-        </is>
-      </c>
-      <c r="D11" t="n">
+      <c r="B11">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11">
         <v>101.6</v>
       </c>
-      <c r="E11" t="n">
+      <c r="E11">
         <v>101.6</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" s="0" outlineLevel="0">
-      <c r="A12" t="n">
+      <c r="F11" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" t="n">
+      <c r="B12">
         <v>5.3</v>
       </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>F</t>
-        </is>
-      </c>
-      <c r="D12" t="n">
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12">
         <v>111.8</v>
       </c>
-      <c r="E12" t="n">
+      <c r="E12">
         <v>111.8</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" s="0" outlineLevel="0">
-      <c r="A13" t="n">
+      <c r="F12" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" t="n">
+      <c r="B13">
         <v>14.5</v>
       </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="D13" t="n">
-        <v>165.0</v>
-      </c>
-      <c r="E13" t="n">
-        <v>165.0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" s="0" outlineLevel="0">
-      <c r="A14" t="n">
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13">
+        <v>165</v>
+      </c>
+      <c r="E13">
+        <v>165</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" t="n">
-        <v>4.4</v>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="D14" t="n">
+      <c r="B14">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14">
         <v>104.1</v>
       </c>
-      <c r="E14" t="n">
+      <c r="E14">
         <v>104.1</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" s="0" outlineLevel="0">
-      <c r="A15" t="n">
+      <c r="F14" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" t="n">
+      <c r="B15">
         <v>12.1</v>
       </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>F</t>
-        </is>
-      </c>
-      <c r="D15" t="n">
-        <v>147.3</v>
-      </c>
-      <c r="E15" t="n">
-        <v>147.3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" s="0" outlineLevel="0">
-      <c r="A16" t="n">
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15">
+        <v>147.30000000000001</v>
+      </c>
+      <c r="E15">
+        <v>147.30000000000001</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" t="n">
+      <c r="B16">
         <v>15.4</v>
       </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="D16" t="n">
+      <c r="C16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16">
         <v>171.5</v>
       </c>
-      <c r="E16" t="n">
+      <c r="E16">
         <v>171.5</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" s="0" outlineLevel="0">
-      <c r="A17" t="n">
+      <c r="F16" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" t="n">
-        <v>16.6</v>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>F</t>
-        </is>
-      </c>
-      <c r="D17" t="n">
+      <c r="B17">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="C17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17">
         <v>161.5</v>
       </c>
-      <c r="E17" t="n">
+      <c r="E17">
         <v>161.5</v>
       </c>
     </row>
@@ -693,22 +819,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>